<commit_message>
weight measurement exp2 02-06
</commit_message>
<xml_diff>
--- a/young-DSS-exp2/weight_measurement.xlsx
+++ b/young-DSS-exp2/weight_measurement.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804FAFC1-ACD5-40E9-BBFE-2FEC3FA2824E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F08512-22BF-41C2-8F03-D58A7B6445FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="31">
   <si>
     <t>Tag</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Birth</t>
+  </si>
+  <si>
+    <t>t28</t>
   </si>
 </sst>
 </file>
@@ -577,15 +580,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -622,8 +625,11 @@
       <c r="L1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>27171</v>
       </c>
@@ -658,8 +664,11 @@
       <c r="L2" s="35">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M2" s="35">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>27123</v>
       </c>
@@ -696,8 +705,11 @@
       <c r="L3" s="35">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>27190</v>
       </c>
@@ -734,8 +746,11 @@
       <c r="L4" s="35">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M4" s="35">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>27161</v>
       </c>
@@ -770,8 +785,11 @@
       <c r="L5" s="35">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M5" s="35">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>27135</v>
       </c>
@@ -806,8 +824,11 @@
       <c r="L6" s="35">
         <v>17.2</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M6" s="35">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>27193</v>
       </c>
@@ -844,8 +865,11 @@
       <c r="L7" s="35">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M7" s="35">
+        <v>17.399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>27125</v>
       </c>
@@ -882,8 +906,11 @@
       <c r="L8" s="35">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M8" s="35">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>27181</v>
       </c>
@@ -918,8 +945,11 @@
       <c r="L9" s="35">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M9" s="35">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>27162</v>
       </c>
@@ -956,8 +986,11 @@
       <c r="L10" s="35">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M10" s="35">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>27126</v>
       </c>
@@ -994,8 +1027,11 @@
       <c r="L11" s="35">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M11" s="35">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>27164</v>
       </c>
@@ -1032,8 +1068,11 @@
       <c r="L12" s="35">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M12" s="35">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>27116</v>
       </c>
@@ -1068,8 +1107,11 @@
       <c r="L13" s="35">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M13" s="35">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>27191</v>
       </c>
@@ -1106,8 +1148,11 @@
       <c r="L14" s="35">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M14" s="35">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>27130</v>
       </c>
@@ -1144,8 +1189,11 @@
       <c r="L15" s="35">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M15" s="35">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>27149</v>
       </c>
@@ -1180,8 +1228,11 @@
       <c r="L16" s="35">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M16" s="35">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>27118</v>
       </c>
@@ -1218,8 +1269,11 @@
       <c r="L17" s="35">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M17" s="35">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>27151</v>
       </c>
@@ -1256,8 +1310,11 @@
       <c r="L18" s="35">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M18" s="35">
+        <v>21.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>27182</v>
       </c>
@@ -1294,8 +1351,11 @@
       <c r="L19" s="35">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M19" s="35">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>27165</v>
       </c>
@@ -1332,8 +1392,11 @@
       <c r="L20" s="35">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M20" s="35">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>27136</v>
       </c>
@@ -1370,8 +1433,11 @@
       <c r="L21" s="35">
         <v>16.600000000000001</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M21" s="35">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>27122</v>
       </c>
@@ -1406,8 +1472,11 @@
       <c r="L22" s="35">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M22" s="35">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>27143</v>
       </c>
@@ -1444,8 +1513,11 @@
       <c r="L23" s="35">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M23" s="35">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>27189</v>
       </c>
@@ -1480,8 +1552,11 @@
       <c r="L24" s="35">
         <v>16.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M24" s="35">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>27128</v>
       </c>
@@ -1518,8 +1593,11 @@
       <c r="L25" s="35">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M25" s="35">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>27163</v>
       </c>
@@ -1556,8 +1634,11 @@
       <c r="L26" s="35">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M26" s="35">
+        <v>18.899999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>27144</v>
       </c>
@@ -1594,8 +1675,11 @@
       <c r="L27" s="35">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M27" s="35">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>27117</v>
       </c>
@@ -1632,8 +1716,11 @@
       <c r="L28" s="35">
         <v>17.7</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M28" s="35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>27127</v>
       </c>
@@ -1668,8 +1755,11 @@
       <c r="L29" s="35">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M29" s="35">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>27150</v>
       </c>
@@ -1706,8 +1796,11 @@
       <c r="L30" s="35">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M30" s="35">
+        <v>19.3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>27192</v>
       </c>
@@ -1744,8 +1837,11 @@
       <c r="L31" s="35">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M31" s="35">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>27172</v>
       </c>
@@ -1782,8 +1878,11 @@
       <c r="L32" s="35">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="M32" s="35">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>27124</v>
       </c>
@@ -1819,6 +1918,9 @@
       </c>
       <c r="L33" s="35">
         <v>18</v>
+      </c>
+      <c r="M33" s="35">
+        <v>18.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>